<commit_message>
Adiciona novas simulações e script para verificar a estrutura da aba Estatisticas_por_Portaria
</commit_message>
<xml_diff>
--- a/output/Entradas-28-10-2025.xlsx
+++ b/output/Entradas-28-10-2025.xlsx
@@ -82682,7 +82682,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN9"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -82694,42 +82694,14 @@
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="26" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
-    <col width="24" customWidth="1" min="7" max="7"/>
-    <col width="29" customWidth="1" min="8" max="8"/>
-    <col width="30" customWidth="1" min="9" max="9"/>
-    <col width="30" customWidth="1" min="10" max="10"/>
-    <col width="30" customWidth="1" min="11" max="11"/>
-    <col width="30" customWidth="1" min="12" max="12"/>
-    <col width="29" customWidth="1" min="13" max="13"/>
-    <col width="30" customWidth="1" min="14" max="14"/>
-    <col width="30" customWidth="1" min="15" max="15"/>
-    <col width="30" customWidth="1" min="16" max="16"/>
-    <col width="28" customWidth="1" min="17" max="17"/>
-    <col width="28" customWidth="1" min="18" max="18"/>
-    <col width="26" customWidth="1" min="19" max="19"/>
-    <col width="30" customWidth="1" min="20" max="20"/>
-    <col width="30" customWidth="1" min="21" max="21"/>
-    <col width="30" customWidth="1" min="22" max="22"/>
-    <col width="30" customWidth="1" min="23" max="23"/>
-    <col width="30" customWidth="1" min="24" max="24"/>
-    <col width="29" customWidth="1" min="25" max="25"/>
-    <col width="30" customWidth="1" min="26" max="26"/>
-    <col width="30" customWidth="1" min="27" max="27"/>
-    <col width="30" customWidth="1" min="28" max="28"/>
-    <col width="29" customWidth="1" min="29" max="29"/>
-    <col width="29" customWidth="1" min="30" max="30"/>
-    <col width="27" customWidth="1" min="31" max="31"/>
-    <col width="30" customWidth="1" min="32" max="32"/>
-    <col width="30" customWidth="1" min="33" max="33"/>
-    <col width="30" customWidth="1" min="34" max="34"/>
-    <col width="30" customWidth="1" min="35" max="35"/>
-    <col width="30" customWidth="1" min="36" max="36"/>
-    <col width="29" customWidth="1" min="37" max="37"/>
-    <col width="30" customWidth="1" min="38" max="38"/>
-    <col width="30" customWidth="1" min="39" max="39"/>
-    <col width="30" customWidth="1" min="40" max="40"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -82755,182 +82727,42 @@
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Port_1_Anexo_I_Registros</t>
+          <t>IDE_Portaria</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Port_1_Anexo_I_Sugestoes</t>
+          <t>Descricao_Portaria</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Port_1_Anexo_I_Acertos</t>
+          <t>Total_Registros</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Port_1_Anexo_I_Precisao_Pct</t>
+          <t>Total_Sugestoes</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Port_1_Anexo_I_Cobertura_Pct</t>
+          <t>Total_Acertos</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Port_1_Anexo_I_Eficiencia_F1</t>
+          <t>Precisao_Pct</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>Port_2_Anexo_II_-_A_Registros</t>
+          <t>Cobertura_Pct</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>Port_2_Anexo_II_-_A_Sugestoes</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>Port_2_Anexo_II_-_A_Acertos</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>Port_2_Anexo_II_-_A_Precisao_Pct</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="inlineStr">
-        <is>
-          <t>Port_2_Anexo_II_-_A_Cobertura_Pct</t>
-        </is>
-      </c>
-      <c r="P1" s="2" t="inlineStr">
-        <is>
-          <t>Port_2_Anexo_II_-_A_Eficiencia_F1</t>
-        </is>
-      </c>
-      <c r="Q1" s="2" t="inlineStr">
-        <is>
-          <t>Port_3_Anexo_III_Registros</t>
-        </is>
-      </c>
-      <c r="R1" s="2" t="inlineStr">
-        <is>
-          <t>Port_3_Anexo_III_Sugestoes</t>
-        </is>
-      </c>
-      <c r="S1" s="2" t="inlineStr">
-        <is>
-          <t>Port_3_Anexo_III_Acertos</t>
-        </is>
-      </c>
-      <c r="T1" s="2" t="inlineStr">
-        <is>
-          <t>Port_3_Anexo_III_Precisao_Pct</t>
-        </is>
-      </c>
-      <c r="U1" s="2" t="inlineStr">
-        <is>
-          <t>Port_3_Anexo_III_Cobertura_Pct</t>
-        </is>
-      </c>
-      <c r="V1" s="2" t="inlineStr">
-        <is>
-          <t>Port_3_Anexo_III_Eficiencia_F1</t>
-        </is>
-      </c>
-      <c r="W1" s="2" t="inlineStr">
-        <is>
-          <t>Port_4_Anexo_IV_-_A_Registros</t>
-        </is>
-      </c>
-      <c r="X1" s="2" t="inlineStr">
-        <is>
-          <t>Port_4_Anexo_IV_-_A_Sugestoes</t>
-        </is>
-      </c>
-      <c r="Y1" s="2" t="inlineStr">
-        <is>
-          <t>Port_4_Anexo_IV_-_A_Acertos</t>
-        </is>
-      </c>
-      <c r="Z1" s="2" t="inlineStr">
-        <is>
-          <t>Port_4_Anexo_IV_-_A_Precisao_Pct</t>
-        </is>
-      </c>
-      <c r="AA1" s="2" t="inlineStr">
-        <is>
-          <t>Port_4_Anexo_IV_-_A_Cobertura_Pct</t>
-        </is>
-      </c>
-      <c r="AB1" s="2" t="inlineStr">
-        <is>
-          <t>Port_4_Anexo_IV_-_A_Eficiencia_F1</t>
-        </is>
-      </c>
-      <c r="AC1" s="2" t="inlineStr">
-        <is>
-          <t>Port_5_Chapelaria_Registros</t>
-        </is>
-      </c>
-      <c r="AD1" s="2" t="inlineStr">
-        <is>
-          <t>Port_5_Chapelaria_Sugestoes</t>
-        </is>
-      </c>
-      <c r="AE1" s="2" t="inlineStr">
-        <is>
-          <t>Port_5_Chapelaria_Acertos</t>
-        </is>
-      </c>
-      <c r="AF1" s="2" t="inlineStr">
-        <is>
-          <t>Port_5_Chapelaria_Precisao_Pct</t>
-        </is>
-      </c>
-      <c r="AG1" s="2" t="inlineStr">
-        <is>
-          <t>Port_5_Chapelaria_Cobertura_Pct</t>
-        </is>
-      </c>
-      <c r="AH1" s="2" t="inlineStr">
-        <is>
-          <t>Port_5_Chapelaria_Eficiencia_F1</t>
-        </is>
-      </c>
-      <c r="AI1" s="2" t="inlineStr">
-        <is>
-          <t>Port_8_Anexo_IV_-_G_Registros</t>
-        </is>
-      </c>
-      <c r="AJ1" s="2" t="inlineStr">
-        <is>
-          <t>Port_8_Anexo_IV_-_G_Sugestoes</t>
-        </is>
-      </c>
-      <c r="AK1" s="2" t="inlineStr">
-        <is>
-          <t>Port_8_Anexo_IV_-_G_Acertos</t>
-        </is>
-      </c>
-      <c r="AL1" s="2" t="inlineStr">
-        <is>
-          <t>Port_8_Anexo_IV_-_G_Precisao_Pct</t>
-        </is>
-      </c>
-      <c r="AM1" s="2" t="inlineStr">
-        <is>
-          <t>Port_8_Anexo_IV_-_G_Cobertura_Pct</t>
-        </is>
-      </c>
-      <c r="AN1" s="2" t="inlineStr">
-        <is>
-          <t>Port_8_Anexo_IV_-_G_Eficiencia_F1</t>
+          <t>Eficiencia_F1</t>
         </is>
       </c>
     </row>
@@ -82952,265 +82784,103 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>590</v>
-      </c>
-      <c r="L2" t="n">
-        <v>32</v>
-      </c>
-      <c r="M2" t="n">
-        <v>19</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>59.4</v>
-      </c>
-      <c r="O2" s="4" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="P2" s="4" t="n">
-        <v>9.9</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>252</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>206</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
+      <c r="J2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Simulação 2</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Simulação 2</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>590</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>590</v>
-      </c>
-      <c r="L3" t="n">
-        <v>73</v>
-      </c>
-      <c r="M3" t="n">
-        <v>32</v>
-      </c>
-      <c r="N3" s="5" t="n">
-        <v>43.8</v>
-      </c>
-      <c r="O3" s="4" t="n">
-        <v>12.4</v>
-      </c>
-      <c r="P3" s="4" t="n">
-        <v>19.3</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>252</v>
-      </c>
-      <c r="R3" t="n">
-        <v>4</v>
-      </c>
-      <c r="S3" t="n">
-        <v>4</v>
-      </c>
-      <c r="T3" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="U3" s="4" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="V3" s="4" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="W3" t="n">
-        <v>206</v>
-      </c>
-      <c r="X3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="AA3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="4" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>59.4</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>9.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Simulação 3</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Simulação 3</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -83218,125 +82888,43 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>590</v>
-      </c>
-      <c r="L4" t="n">
-        <v>149</v>
-      </c>
-      <c r="M4" t="n">
-        <v>52</v>
-      </c>
-      <c r="N4" s="5" t="n">
-        <v>34.9</v>
-      </c>
-      <c r="O4" s="4" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="P4" s="3" t="n">
-        <v>29.3</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>252</v>
-      </c>
-      <c r="R4" t="n">
-        <v>30</v>
-      </c>
-      <c r="S4" t="n">
-        <v>19</v>
-      </c>
-      <c r="T4" s="5" t="n">
-        <v>63.3</v>
-      </c>
-      <c r="U4" s="4" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="V4" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="W4" t="n">
-        <v>206</v>
-      </c>
-      <c r="X4" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z4" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="AA4" s="4" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="AB4" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
+      <c r="J4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Simulação 4</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Simulação 4</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -83344,113 +82932,29 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>590</v>
-      </c>
-      <c r="L5" t="n">
-        <v>208</v>
-      </c>
-      <c r="M5" t="n">
-        <v>62</v>
-      </c>
-      <c r="N5" s="4" t="n">
-        <v>29.8</v>
-      </c>
-      <c r="O5" s="5" t="n">
-        <v>35.3</v>
-      </c>
-      <c r="P5" s="3" t="n">
-        <v>32.3</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>252</v>
-      </c>
-      <c r="R5" t="n">
-        <v>44</v>
-      </c>
-      <c r="S5" t="n">
-        <v>27</v>
-      </c>
-      <c r="T5" s="5" t="n">
-        <v>61.4</v>
-      </c>
-      <c r="U5" s="5" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="V5" s="5" t="n">
-        <v>27.2</v>
-      </c>
-      <c r="W5" t="n">
-        <v>206</v>
-      </c>
-      <c r="X5" t="n">
-        <v>24</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>13</v>
-      </c>
-      <c r="Z5" s="3" t="n">
-        <v>54.2</v>
-      </c>
-      <c r="AA5" s="4" t="n">
-        <v>11.7</v>
-      </c>
-      <c r="AB5" s="4" t="n">
-        <v>19.2</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
+      <c r="J5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Simulação 5</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Simulação 5</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
         <v>10</v>
@@ -83458,11 +82962,13 @@
       <c r="E6" t="n">
         <v>5</v>
       </c>
-      <c r="F6" t="n">
-        <v>0</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -83470,125 +82976,43 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>590</v>
-      </c>
-      <c r="L6" t="n">
-        <v>312</v>
-      </c>
-      <c r="M6" t="n">
-        <v>84</v>
-      </c>
-      <c r="N6" s="4" t="n">
-        <v>26.9</v>
-      </c>
-      <c r="O6" s="5" t="n">
-        <v>52.9</v>
-      </c>
-      <c r="P6" s="3" t="n">
-        <v>35.7</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>252</v>
-      </c>
-      <c r="R6" t="n">
-        <v>57</v>
-      </c>
-      <c r="S6" t="n">
-        <v>33</v>
-      </c>
-      <c r="T6" s="5" t="n">
-        <v>57.9</v>
-      </c>
-      <c r="U6" s="5" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="V6" s="3" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="W6" t="n">
-        <v>206</v>
-      </c>
-      <c r="X6" t="n">
-        <v>67</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>44</v>
-      </c>
-      <c r="Z6" s="3" t="n">
-        <v>65.7</v>
-      </c>
-      <c r="AA6" s="5" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="AB6" s="5" t="n">
-        <v>43.5</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
+      <c r="J6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Simulação 6</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Simulação 6</t>
+          <t>Simulação 1</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" t="n">
         <v>8</v>
       </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -83596,354 +83020,1866 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>590</v>
-      </c>
-      <c r="L7" t="n">
-        <v>452</v>
-      </c>
-      <c r="M7" t="n">
-        <v>98</v>
-      </c>
-      <c r="N7" s="4" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="O7" s="3" t="n">
-        <v>76.59999999999999</v>
-      </c>
-      <c r="P7" s="3" t="n">
-        <v>33.8</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>252</v>
-      </c>
-      <c r="R7" t="n">
-        <v>105</v>
-      </c>
-      <c r="S7" t="n">
-        <v>54</v>
-      </c>
-      <c r="T7" s="5" t="n">
-        <v>51.4</v>
-      </c>
-      <c r="U7" s="3" t="n">
-        <v>41.7</v>
-      </c>
-      <c r="V7" s="3" t="n">
-        <v>46</v>
-      </c>
-      <c r="W7" t="n">
-        <v>206</v>
-      </c>
-      <c r="X7" t="n">
-        <v>128</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>81</v>
-      </c>
-      <c r="Z7" s="3" t="n">
-        <v>63.3</v>
-      </c>
-      <c r="AA7" s="3" t="n">
-        <v>62.1</v>
-      </c>
-      <c r="AB7" s="3" t="n">
-        <v>62.7</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="n">
+      <c r="J7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Simulação 7</t>
+          <t>Simulação 2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Simulação 7</t>
+          <t>Simulação 2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
         <v>5</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>590</v>
-      </c>
-      <c r="L8" t="n">
-        <v>382</v>
-      </c>
-      <c r="M8" t="n">
-        <v>76</v>
-      </c>
-      <c r="N8" s="4" t="n">
-        <v>19.9</v>
-      </c>
-      <c r="O8" s="3" t="n">
-        <v>64.7</v>
-      </c>
-      <c r="P8" s="3" t="n">
-        <v>30.4</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>252</v>
-      </c>
-      <c r="R8" t="n">
-        <v>91</v>
-      </c>
-      <c r="S8" t="n">
-        <v>51</v>
-      </c>
-      <c r="T8" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="U8" s="3" t="n">
-        <v>36.1</v>
-      </c>
-      <c r="V8" s="3" t="n">
-        <v>43.9</v>
-      </c>
-      <c r="W8" t="n">
-        <v>206</v>
-      </c>
-      <c r="X8" t="n">
-        <v>115</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>71</v>
-      </c>
-      <c r="Z8" s="3" t="n">
-        <v>61.7</v>
-      </c>
-      <c r="AA8" s="3" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="AB8" s="3" t="n">
-        <v>58.6</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>44</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>17</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="n">
+      <c r="J8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>590</v>
+      </c>
+      <c r="H9" t="n">
+        <v>73</v>
+      </c>
+      <c r="I9" t="n">
+        <v>32</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>43.8</v>
+      </c>
+      <c r="K9" s="4" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>252</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="K10" s="4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>206</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="K11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>44</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Simulação 2</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>17</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>15</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>10</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>590</v>
+      </c>
+      <c r="H15" t="n">
+        <v>149</v>
+      </c>
+      <c r="I15" t="n">
+        <v>52</v>
+      </c>
+      <c r="J15" s="4" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>252</v>
+      </c>
+      <c r="H16" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="n">
+        <v>19</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>63.3</v>
+      </c>
+      <c r="K16" s="4" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="L16" s="4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>206</v>
+      </c>
+      <c r="H17" t="n">
+        <v>14</v>
+      </c>
+      <c r="I17" t="n">
+        <v>7</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="K17" s="4" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="L17" s="4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>15</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>44</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Simulação 3</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>15</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>20</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>590</v>
+      </c>
+      <c r="H21" t="n">
+        <v>208</v>
+      </c>
+      <c r="I21" t="n">
+        <v>62</v>
+      </c>
+      <c r="J21" s="4" t="n">
+        <v>29.8</v>
+      </c>
+      <c r="K21" s="5" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="L21" s="5" t="n">
+        <v>32.3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>252</v>
+      </c>
+      <c r="H22" t="n">
+        <v>44</v>
+      </c>
+      <c r="I22" t="n">
+        <v>27</v>
+      </c>
+      <c r="J22" s="5" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="K22" s="4" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="L22" s="5" t="n">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>20</v>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>206</v>
+      </c>
+      <c r="H23" t="n">
+        <v>24</v>
+      </c>
+      <c r="I23" t="n">
+        <v>13</v>
+      </c>
+      <c r="J23" s="5" t="n">
+        <v>54.2</v>
+      </c>
+      <c r="K23" s="4" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>20</v>
+      </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>44</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Simulação 4</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>20</v>
+      </c>
+      <c r="D25" t="n">
+        <v>10</v>
+      </c>
+      <c r="E25" t="n">
+        <v>8</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>17</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>30</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>590</v>
+      </c>
+      <c r="H27" t="n">
+        <v>312</v>
+      </c>
+      <c r="I27" t="n">
+        <v>84</v>
+      </c>
+      <c r="J27" s="4" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="K27" s="5" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="L27" s="5" t="n">
+        <v>35.7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>30</v>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>252</v>
+      </c>
+      <c r="H28" t="n">
+        <v>57</v>
+      </c>
+      <c r="I28" t="n">
+        <v>33</v>
+      </c>
+      <c r="J28" s="5" t="n">
+        <v>57.9</v>
+      </c>
+      <c r="K28" s="4" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="L28" s="5" t="n">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>30</v>
+      </c>
+      <c r="D29" t="n">
+        <v>10</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>206</v>
+      </c>
+      <c r="H29" t="n">
+        <v>67</v>
+      </c>
+      <c r="I29" t="n">
+        <v>44</v>
+      </c>
+      <c r="J29" s="5" t="n">
+        <v>65.7</v>
+      </c>
+      <c r="K29" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>30</v>
+      </c>
+      <c r="D30" t="n">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>5</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>44</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Simulação 5</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" t="n">
+        <v>10</v>
+      </c>
+      <c r="E31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>17</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>45</v>
+      </c>
+      <c r="D32" t="n">
+        <v>8</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>5</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>45</v>
+      </c>
+      <c r="D33" t="n">
+        <v>8</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>590</v>
+      </c>
+      <c r="H33" t="n">
+        <v>452</v>
+      </c>
+      <c r="I33" t="n">
+        <v>98</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="L33" s="5" t="n">
+        <v>33.8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>45</v>
+      </c>
+      <c r="D34" t="n">
+        <v>8</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>252</v>
+      </c>
+      <c r="H34" t="n">
+        <v>105</v>
+      </c>
+      <c r="I34" t="n">
+        <v>54</v>
+      </c>
+      <c r="J34" s="5" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="K34" s="5" t="n">
+        <v>41.7</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>45</v>
+      </c>
+      <c r="D35" t="n">
+        <v>8</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>206</v>
+      </c>
+      <c r="H35" t="n">
+        <v>128</v>
+      </c>
+      <c r="I35" t="n">
+        <v>81</v>
+      </c>
+      <c r="J35" s="5" t="n">
+        <v>63.3</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>62.1</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>62.7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>45</v>
+      </c>
+      <c r="D36" t="n">
+        <v>8</v>
+      </c>
+      <c r="E36" t="n">
+        <v>5</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>44</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Simulação 6</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>45</v>
+      </c>
+      <c r="D37" t="n">
+        <v>8</v>
+      </c>
+      <c r="E37" t="n">
+        <v>8</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>17</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>60</v>
+      </c>
+      <c r="D38" t="n">
+        <v>12</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>5</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>60</v>
+      </c>
+      <c r="D39" t="n">
+        <v>12</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>590</v>
+      </c>
+      <c r="H39" t="n">
+        <v>382</v>
+      </c>
+      <c r="I39" t="n">
+        <v>76</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="L39" s="5" t="n">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>60</v>
+      </c>
+      <c r="D40" t="n">
+        <v>12</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>252</v>
+      </c>
+      <c r="H40" t="n">
+        <v>91</v>
+      </c>
+      <c r="I40" t="n">
+        <v>51</v>
+      </c>
+      <c r="J40" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="K40" s="5" t="n">
+        <v>36.1</v>
+      </c>
+      <c r="L40" s="3" t="n">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>60</v>
+      </c>
+      <c r="D41" t="n">
+        <v>12</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>206</v>
+      </c>
+      <c r="H41" t="n">
+        <v>115</v>
+      </c>
+      <c r="I41" t="n">
+        <v>71</v>
+      </c>
+      <c r="J41" s="5" t="n">
+        <v>61.7</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>60</v>
+      </c>
+      <c r="D42" t="n">
+        <v>12</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>44</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Simulação 7</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>60</v>
+      </c>
+      <c r="D43" t="n">
+        <v>12</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>17</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>Simulação 8</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>Simulação 8</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C44" t="n">
         <v>90</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D44" t="n">
         <v>15</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Anexo I</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
         <v>5</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>90</v>
+      </c>
+      <c r="D45" t="n">
+        <v>15</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Anexo II - A</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
         <v>590</v>
       </c>
-      <c r="L9" t="n">
+      <c r="H45" t="n">
         <v>435</v>
       </c>
-      <c r="M9" t="n">
+      <c r="I45" t="n">
         <v>73</v>
       </c>
-      <c r="N9" s="4" t="n">
+      <c r="J45" s="4" t="n">
         <v>16.8</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="K45" s="3" t="n">
         <v>73.7</v>
       </c>
-      <c r="P9" s="5" t="n">
+      <c r="L45" s="5" t="n">
         <v>27.3</v>
       </c>
-      <c r="Q9" t="n">
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>90</v>
+      </c>
+      <c r="D46" t="n">
+        <v>15</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Anexo III</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
         <v>252</v>
       </c>
-      <c r="R9" t="n">
+      <c r="H46" t="n">
         <v>102</v>
       </c>
-      <c r="S9" t="n">
+      <c r="I46" t="n">
         <v>52</v>
       </c>
-      <c r="T9" s="5" t="n">
+      <c r="J46" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="U9" s="3" t="n">
+      <c r="K46" s="5" t="n">
         <v>40.5</v>
       </c>
-      <c r="V9" s="3" t="n">
+      <c r="L46" s="3" t="n">
         <v>45.1</v>
       </c>
-      <c r="W9" t="n">
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>90</v>
+      </c>
+      <c r="D47" t="n">
+        <v>15</v>
+      </c>
+      <c r="E47" t="n">
+        <v>4</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Anexo IV - A</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
         <v>206</v>
       </c>
-      <c r="X9" t="n">
+      <c r="H47" t="n">
         <v>121</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="I47" t="n">
         <v>70</v>
       </c>
-      <c r="Z9" s="3" t="n">
+      <c r="J47" s="5" t="n">
         <v>57.9</v>
       </c>
-      <c r="AA9" s="3" t="n">
+      <c r="K47" s="3" t="n">
         <v>58.7</v>
       </c>
-      <c r="AB9" s="3" t="n">
+      <c r="L47" s="3" t="n">
         <v>58.3</v>
       </c>
-      <c r="AC9" t="n">
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>90</v>
+      </c>
+      <c r="D48" t="n">
+        <v>15</v>
+      </c>
+      <c r="E48" t="n">
+        <v>5</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Chapelaria</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
         <v>44</v>
       </c>
-      <c r="AD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI9" t="n">
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Simulação 8</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>90</v>
+      </c>
+      <c r="D49" t="n">
+        <v>15</v>
+      </c>
+      <c r="E49" t="n">
+        <v>8</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Anexo IV - G</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
         <v>17</v>
       </c>
-      <c r="AJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="n">
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="4" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="J2:J49">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -83955,7 +84891,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="K2:K49">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -83967,188 +84903,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="L2:L49">
     <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00F1F8E9"/>
-        <color rgb="0066BB6A"/>
-        <color rgb="001B5E20"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N9">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O9">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P9">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00F1F8E9"/>
-        <color rgb="0066BB6A"/>
-        <color rgb="001B5E20"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T9">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U9">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V9">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00F1F8E9"/>
-        <color rgb="0066BB6A"/>
-        <color rgb="001B5E20"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z9">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA9">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB9">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00F1F8E9"/>
-        <color rgb="0066BB6A"/>
-        <color rgb="001B5E20"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF2:AF9">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG9">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH9">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00F1F8E9"/>
-        <color rgb="0066BB6A"/>
-        <color rgb="001B5E20"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL2:AL9">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM9">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="00E8F5E8"/>
-        <color rgb="00A8D8A8"/>
-        <color rgb="002E7D32"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN2:AN9">
-    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>